<commit_message>
Update Dashboard Analisando dados de clientes.xlsx
</commit_message>
<xml_diff>
--- a/Dashboard Analisando dados de clientes.xlsx
+++ b/Dashboard Analisando dados de clientes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOME\Documents\GitHub\Meus-Projetos-de-Análise-de-Dados\Analisando dados de vendas e clientes com SQL e Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOME\Documents\GitHub\Analisando-dados-de-vendas-e-clientes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C0BDE9-1459-4A2A-B7CB-D1002A1BFAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196E4506-BC1F-43CC-96D7-A191A02124B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DE66B0D5-D4DC-4560-A9A8-B6EB22104F2E}"/>
   </bookViews>

</xml_diff>